<commit_message>
experiment design changes PB/RW
</commit_message>
<xml_diff>
--- a/Report material/Experiment design.xlsx
+++ b/Report material/Experiment design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\localdev\RL-final-project\Report material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA5370B1-A75C-4D6D-90E1-6F48E38752FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EF41EA-FC4D-4DA9-8936-115BF76004C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64F49380-DFF0-40C2-9764-7D95B8F44442}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="61">
   <si>
     <t>size of field</t>
   </si>
@@ -189,9 +189,6 @@
     <t>Fixed at 1</t>
   </si>
   <si>
-    <t>Fixed at ?</t>
-  </si>
-  <si>
     <t>Q table init: zeros (0) or optimistic (+1 tbd), or random small values</t>
   </si>
   <si>
@@ -208,6 +205,18 @@
   </si>
   <si>
     <t>In hunting scenarios: higher alpha is better</t>
+  </si>
+  <si>
+    <t>ENV6</t>
+  </si>
+  <si>
+    <t>ENV7</t>
+  </si>
+  <si>
+    <t>ENV8</t>
+  </si>
+  <si>
+    <t>Fixed at 1?</t>
   </si>
 </sst>
 </file>
@@ -239,7 +248,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,6 +258,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -265,11 +304,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -584,58 +628,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{804BF346-908A-4FAF-AA6C-CF500CD359E0}">
-  <dimension ref="C2:L46"/>
+  <dimension ref="C2:O46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="26.85546875" customWidth="1"/>
     <col min="4" max="4" width="34" customWidth="1"/>
-    <col min="5" max="10" width="9.5703125" customWidth="1"/>
-    <col min="11" max="13" width="13" customWidth="1"/>
+    <col min="5" max="13" width="9.5703125" customWidth="1"/>
+    <col min="14" max="16" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>25</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>27</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>28</v>
       </c>
@@ -643,7 +690,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
@@ -662,52 +709,70 @@
       <c r="I10" t="s">
         <v>38</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="J10" t="s">
+        <v>57</v>
+      </c>
+      <c r="K10" t="s">
+        <v>58</v>
+      </c>
+      <c r="L10" t="s">
+        <v>59</v>
+      </c>
+      <c r="O10" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>49</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="L12" t="s">
+      <c r="K12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="O12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="L13" t="s">
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="L14" t="s">
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="L15" t="s">
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>7</v>
       </c>
@@ -717,24 +782,27 @@
       <c r="E16" t="s">
         <v>39</v>
       </c>
-      <c r="L16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>39</v>
+      </c>
+      <c r="O16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L17" t="s">
+      <c r="O17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="L18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>29</v>
       </c>
@@ -744,47 +812,65 @@
       <c r="E19" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>31</v>
       </c>
       <c r="E21" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>32</v>
       </c>
       <c r="E23" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>6</v>
       </c>
       <c r="D26" t="s">
         <v>1</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K26" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="I26" t="s">
+      <c r="L26" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>12</v>
       </c>
@@ -794,18 +880,21 @@
       <c r="E28" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>11</v>
       </c>
@@ -815,14 +904,29 @@
       <c r="E32" t="s">
         <v>43</v>
       </c>
+      <c r="F32" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="G32" t="s">
+        <v>43</v>
+      </c>
+      <c r="H32" s="6" t="s">
         <v>46</v>
       </c>
       <c r="I32" t="s">
+        <v>43</v>
+      </c>
+      <c r="J32" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>43</v>
+      </c>
+      <c r="L32" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>5</v>
       </c>
@@ -832,48 +936,51 @@
       <c r="E34" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
         <v>14</v>
       </c>

</xml_diff>